<commit_message>
v1.2.0; updated dependencies excel sheet
</commit_message>
<xml_diff>
--- a/documentation/Dependencies.xlsx
+++ b/documentation/Dependencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba4eb5\Desktop\Skalierung\Skalierungspaket\scaling\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F796669A-8519-4384-B2B8-072A5B380DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9A063A-FB45-4A13-A925-35BE1998D4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FFCF87-98C9-4C4C-9C88-8C4AFB5511E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Package</t>
   </si>
@@ -74,9 +74,6 @@
     <t>mv_person</t>
   </si>
   <si>
-    <t>utils-pipe</t>
-  </si>
-  <si>
     <t>utils</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>haven</t>
   </si>
   <si>
-    <t>magrittr</t>
-  </si>
-  <si>
     <t>openxlsx</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>tidyselect</t>
   </si>
   <si>
-    <t>magrittr pipe</t>
-  </si>
-  <si>
     <t>oft</t>
   </si>
   <si>
@@ -146,12 +137,6 @@
     <t>sequential_hcl()</t>
   </si>
   <si>
-    <t>zap_labels()</t>
-  </si>
-  <si>
-    <t>used function(s)</t>
-  </si>
-  <si>
     <t>r default load</t>
   </si>
   <si>
@@ -210,6 +195,9 @@
   </si>
   <si>
     <t>oft benutzt und wichtig für scaling Paket</t>
+  </si>
+  <si>
+    <t>single used function</t>
   </si>
 </sst>
 </file>
@@ -288,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,18 +285,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,10 +298,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -655,48 +637,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA4D359-F5EF-4691-98F5-219447C270FB}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="15.7109375" customWidth="1"/>
+    <col min="1" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -733,14 +716,11 @@
       <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -759,14 +739,13 @@
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="R4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -784,16 +763,15 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -805,70 +783,67 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    </row>
+    <row r="7" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10">
+        <v>2</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13">
-        <v>2</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
+        <v>3</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13">
-        <v>3</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -879,281 +854,264 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="R9" s="1" t="s">
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
+        <v>6</v>
+      </c>
+      <c r="M10" s="3">
+        <v>5</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="Q10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="Q12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="Q13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8">
+        <v>3</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="Q16" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="Q17" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5">
+        <v>2</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1</v>
+      </c>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="Q18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14">
-        <v>6</v>
-      </c>
-      <c r="M10" s="14">
-        <v>5</v>
-      </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="R10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9">
-        <v>1</v>
-      </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-    </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2">
-        <v>2</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7">
-        <v>2</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="R13" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="R14" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11">
-        <v>1</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11">
-        <v>3</v>
-      </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11">
-        <v>1</v>
-      </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2">
-        <v>2</v>
-      </c>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="R17" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7">
-        <v>1</v>
-      </c>
-      <c r="M18" s="7">
-        <v>1</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="R18" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7">
-        <v>2</v>
-      </c>
-      <c r="M19" s="7">
-        <v>1</v>
-      </c>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="R19" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1167,110 +1125,56 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="13"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="B29" t="s">
         <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>